<commit_message>
homologacion de modulo -en linea- para campañas complementarias IW
</commit_message>
<xml_diff>
--- a/portal/repositorio/SAVORY/estado_ipt_savory.xlsx
+++ b/portal/repositorio/SAVORY/estado_ipt_savory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8222668d6376a54f/Mentecreativa/Power BI/2 - PANELES BI/SAVORY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_E47DD134F7C84CB72636FBF4962BAA0081A31848" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4779CEF9-EDF1-4E2F-B82D-501C0A913C37}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_E47DD134F7C84CB72636FBF4962BAA0081A31848" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{884E31CF-A9AA-4BE4-B3E2-685C9F1E58F8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,51 +101,6 @@
     <t>ZONA</t>
   </si>
   <si>
-    <t>R01</t>
-  </si>
-  <si>
-    <t>R02</t>
-  </si>
-  <si>
-    <t>R03</t>
-  </si>
-  <si>
-    <t>R04</t>
-  </si>
-  <si>
-    <t>R05</t>
-  </si>
-  <si>
-    <t>R06</t>
-  </si>
-  <si>
-    <t>R07</t>
-  </si>
-  <si>
-    <t>R09</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>SAMKA</t>
-  </si>
-  <si>
-    <t>IGNAMAR</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>ARAZA</t>
-  </si>
-  <si>
-    <t>DIMER</t>
-  </si>
-  <si>
-    <t>ICEFREE</t>
-  </si>
-  <si>
     <t>TIPO DE ZONA</t>
   </si>
   <si>
@@ -158,9 +113,6 @@
     <t>DISTRIBUIDOR</t>
   </si>
   <si>
-    <t>ONIX</t>
-  </si>
-  <si>
     <t>DIRECTA</t>
   </si>
   <si>
@@ -170,33 +122,18 @@
     <t>SAN FELIPE</t>
   </si>
   <si>
-    <t>FRISUR</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
-    <t>GYG</t>
-  </si>
-  <si>
     <t>CHILLAN</t>
   </si>
   <si>
-    <t>R08</t>
-  </si>
-  <si>
     <t>GGORMAZ</t>
   </si>
   <si>
     <t>FGALLARDO</t>
   </si>
   <si>
-    <t>GIANTCOLD</t>
-  </si>
-  <si>
-    <t>DIANSE</t>
-  </si>
-  <si>
     <t>LOS ANGELES/CHILLAN</t>
   </si>
   <si>
@@ -216,6 +153,69 @@
   </si>
   <si>
     <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>SAMKA - IQUIQUE</t>
+  </si>
+  <si>
+    <t>ARAZA - ANTOFAGASTA</t>
+  </si>
+  <si>
+    <t>R1 - LA SERENA</t>
+  </si>
+  <si>
+    <t>ONIX - COPIAPÓ</t>
+  </si>
+  <si>
+    <t>DIMER - VIÑA DEL MAR</t>
+  </si>
+  <si>
+    <t>IGNAMAR - ALGARROBO</t>
+  </si>
+  <si>
+    <t>R2 - SANTIAGO CENTRO</t>
+  </si>
+  <si>
+    <t>R3 - SANTIAGO SUR</t>
+  </si>
+  <si>
+    <t>R4 - SANTIAGO ORIENTE</t>
+  </si>
+  <si>
+    <t>R5 - SANTIAGO PONIENTE</t>
+  </si>
+  <si>
+    <t>R6 - SANTIAGO SURORIENTE</t>
+  </si>
+  <si>
+    <t>ICE FREE</t>
+  </si>
+  <si>
+    <t>R7 - RANCAGUA / SAN VICENTE</t>
+  </si>
+  <si>
+    <t>G&amp;G - TALCA</t>
+  </si>
+  <si>
+    <t>R8 - LOS ANGELES / CHILLAN</t>
+  </si>
+  <si>
+    <t>GIANTCOLD - CHILLÁN</t>
+  </si>
+  <si>
+    <t>R9 - CONCEPCIÓN</t>
+  </si>
+  <si>
+    <t>R10 - TEMUCO/VALDIVIA</t>
+  </si>
+  <si>
+    <t>DIANSE - TEMUCO</t>
+  </si>
+  <si>
+    <t>R11 - PTO MONTT</t>
+  </si>
+  <si>
+    <t>EN PAUSA</t>
   </si>
 </sst>
 </file>
@@ -421,16 +421,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,6 +447,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,21 +773,23 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -792,15 +798,15 @@
         <v>21</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -809,98 +815,98 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E2" s="17">
-        <v>46031</v>
+        <v>46038</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E3" s="17">
-        <v>46031</v>
+        <v>46041</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="18">
-        <v>46031</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>2</v>
+        <v>46035</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="17">
-        <v>46031</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="E5" s="18">
+        <v>46011</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E6" s="17">
-        <v>46030</v>
+        <v>46035</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>3</v>
@@ -909,27 +915,27 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E7" s="17">
-        <v>46031</v>
+        <v>46037</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>2</v>
@@ -940,127 +946,127 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="18">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="E10" s="18">
-        <v>46030</v>
+        <v>45980</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E11" s="18">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E12" s="18">
-        <v>46029</v>
+        <v>46034</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E13" s="18">
-        <v>46029</v>
+        <v>46034</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E14" s="20">
         <v>46034</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
@@ -1069,18 +1075,18 @@
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E15" s="17">
-        <v>46029</v>
+        <v>46036</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>19</v>
@@ -1089,58 +1095,58 @@
         <v>18</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E16" s="17">
-        <v>46030</v>
+        <v>46037</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>52</v>
-      </c>
       <c r="E17" s="18">
-        <v>46031</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>2</v>
+        <v>46041</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E18" s="18">
-        <v>46031</v>
+        <v>45996</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>7</v>
@@ -1149,58 +1155,58 @@
         <v>10</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E19" s="17">
-        <v>46030</v>
+        <v>46035</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="E20" s="18">
-        <v>46031</v>
+        <v>46037</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E21" s="18">
-        <v>46031</v>
+        <v>46037</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>9</v>
@@ -1209,13 +1215,13 @@
         <v>8</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E22" s="17">
-        <v>46031</v>
+        <v>46038</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>